<commit_message>
Javadocs, Unit Tests, and last global corrections
</commit_message>
<xml_diff>
--- a/PI-2023-24 Self-Assessment.xlsx
+++ b/PI-2023-24 Self-Assessment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rui Silva\Desktop\Work\lapr\lei-24-s2-1dkl-g134\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1F5238-E5DD-4343-9970-11A866170ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7B254B-0591-451E-B459-5A8258A54647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1764,8 +1764,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1799,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="6">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
@@ -1908,19 +1908,19 @@
         <v>1231105</v>
       </c>
       <c r="D10" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="38">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" s="39">
         <v>4</v>
       </c>
       <c r="G10" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10" s="39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
@@ -1943,16 +1943,16 @@
         <v>1231138</v>
       </c>
       <c r="D11" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" s="35">
         <v>4</v>
       </c>
       <c r="G11" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11" s="8">
         <v>4</v>
@@ -1969,7 +1969,7 @@
       <c r="R11" s="10"/>
       <c r="S11" s="51">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1981,16 +1981,16 @@
         <v>5</v>
       </c>
       <c r="E12" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F12" s="36">
+        <v>5</v>
+      </c>
+      <c r="G12" s="35">
         <v>3</v>
       </c>
-      <c r="G12" s="35">
-        <v>4</v>
-      </c>
       <c r="H12" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -2004,7 +2004,7 @@
       <c r="R12" s="10"/>
       <c r="S12" s="51">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2013,19 +2013,19 @@
         <v>1230665</v>
       </c>
       <c r="D13" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E13" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" s="9">
         <v>4</v>
       </c>
       <c r="G13" s="36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H13" s="35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
@@ -2048,16 +2048,16 @@
         <v>1230573</v>
       </c>
       <c r="D14" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="8">
         <v>4</v>
       </c>
       <c r="G14" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H14" s="36">
         <v>4</v>
@@ -2074,7 +2074,7 @@
       <c r="R14" s="10"/>
       <c r="S14" s="51">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2334,23 +2334,23 @@
       </c>
       <c r="D25" s="46">
         <f>AVERAGE(D10:D24)</f>
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="E25" s="46">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H25" s="46">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I25" s="46" t="e">
         <f t="shared" si="1"/>
@@ -4423,12 +4423,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4616,15 +4613,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4648,17 +4656,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test documentation and self-asessment
</commit_message>
<xml_diff>
--- a/PI-2023-24 Self-Assessment.xlsx
+++ b/PI-2023-24 Self-Assessment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rui Silva\Desktop\Work\lapr\lei-24-s2-1dkl-g134\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7B254B-0591-451E-B459-5A8258A54647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5F76BD-CA61-4C8D-8B14-D0638CE40403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1943,16 +1943,16 @@
         <v>1231138</v>
       </c>
       <c r="D11" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11" s="35">
         <v>4</v>
       </c>
       <c r="G11" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H11" s="8">
         <v>4</v>
@@ -1969,7 +1969,7 @@
       <c r="R11" s="10"/>
       <c r="S11" s="51">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>3.8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1978,19 +1978,19 @@
         <v>1212009</v>
       </c>
       <c r="D12" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" s="36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H12" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -2004,7 +2004,7 @@
       <c r="R12" s="10"/>
       <c r="S12" s="51">
         <f t="shared" si="0"/>
-        <v>4.2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2016,13 +2016,13 @@
         <v>5</v>
       </c>
       <c r="E13" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" s="9">
         <v>4</v>
       </c>
       <c r="G13" s="36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="35">
         <v>5</v>
@@ -2039,7 +2039,7 @@
       <c r="R13" s="10"/>
       <c r="S13" s="51">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2051,13 +2051,13 @@
         <v>5</v>
       </c>
       <c r="E14" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F14" s="8">
         <v>4</v>
       </c>
       <c r="G14" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H14" s="36">
         <v>4</v>
@@ -2074,7 +2074,7 @@
       <c r="R14" s="10"/>
       <c r="S14" s="51">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2334,23 +2334,23 @@
       </c>
       <c r="D25" s="46">
         <f>AVERAGE(D10:D24)</f>
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E25" s="46">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="H25" s="46">
         <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I25" s="46" t="e">
         <f t="shared" si="1"/>
@@ -4423,9 +4423,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4613,26 +4616,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4656,9 +4648,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>